<commit_message>
Changes to html form;changes to server side event messaging;navigation across pages
</commit_message>
<xml_diff>
--- a/files/excel/campaign_input_09122025.xlsx
+++ b/files/excel/campaign_input_09122025.xlsx
@@ -648,7 +648,7 @@
       </c>
       <c r="H5" s="2" t="inlineStr">
         <is>
-          <t>Sent email at slno 1 at time: 11/12/2025,17:21:36</t>
+          <t>Sent email at slno 1 at time: 12/12/2025,20:10:09</t>
         </is>
       </c>
     </row>
@@ -678,7 +678,7 @@
       </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>Sent email at slno 2 at time: 11/12/2025,17:21:44</t>
+          <t>Sent email at slno 2 at time: 12/12/2025,20:10:09</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added logic for tracking url for campaigns
</commit_message>
<xml_diff>
--- a/files/excel/campaign_input_09122025.xlsx
+++ b/files/excel/campaign_input_09122025.xlsx
@@ -648,7 +648,7 @@
       </c>
       <c r="H5" s="2" t="inlineStr">
         <is>
-          <t>Sent email at slno 1 at time: 12/12/2025,20:10:09</t>
+          <t>Sent email at slno 1 at time: 13/12/2025,11:39:13</t>
         </is>
       </c>
     </row>
@@ -678,7 +678,7 @@
       </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>Sent email at slno 2 at time: 12/12/2025,20:10:09</t>
+          <t>Sent email at slno 2 at time: 13/12/2025,11:39:18</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Moved sender credentaials from code to db
</commit_message>
<xml_diff>
--- a/files/excel/campaign_input_09122025.xlsx
+++ b/files/excel/campaign_input_09122025.xlsx
@@ -648,7 +648,7 @@
       </c>
       <c r="H5" s="2" t="inlineStr">
         <is>
-          <t>Sent email at slno 1 at time: 13/12/2025,11:39:13</t>
+          <t>Sent email at slno 1 at time: 08/01/2026,17:50:34</t>
         </is>
       </c>
     </row>
@@ -678,7 +678,7 @@
       </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>Sent email at slno 2 at time: 13/12/2025,11:39:18</t>
+          <t>Sent email at slno 2 at time: 08/01/2026,17:50:38</t>
         </is>
       </c>
     </row>

</xml_diff>